<commit_message>
correccion en excelservice.py, para celdas combinadas
</commit_message>
<xml_diff>
--- a/proforma_final.xlsx
+++ b/proforma_final.xlsx
@@ -1632,7 +1632,7 @@
           <t>UNIDAD</t>
         </is>
       </c>
-      <c r="D18" s="25" t="inlineStr">
+      <c r="D18" s="63" t="inlineStr">
         <is>
           <t>LAMINAS CONTAC FLUORESCENTE A4 NARANJA</t>
         </is>
@@ -1681,11 +1681,11 @@
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B19" s="63" t="n"/>
-      <c r="C19" s="63" t="n"/>
-      <c r="D19" s="63" t="n"/>
-      <c r="E19" s="63" t="n"/>
-      <c r="F19" s="64" t="n"/>
+      <c r="B19" s="23" t="n"/>
+      <c r="C19" s="24" t="n"/>
+      <c r="D19" s="25" t="n"/>
+      <c r="E19" s="26" t="n"/>
+      <c r="F19" s="76" t="n"/>
       <c r="G19" s="77" t="n">
         <v>660</v>
       </c>
@@ -1717,7 +1717,11 @@
       </c>
       <c r="B20" s="63" t="n"/>
       <c r="C20" s="64" t="n"/>
-      <c r="D20" s="87" t="n"/>
+      <c r="D20" s="87" t="inlineStr">
+        <is>
+          <t>10 DÍAS</t>
+        </is>
+      </c>
       <c r="E20" s="63" t="n"/>
       <c r="F20" s="63" t="n"/>
       <c r="G20" s="64" t="n"/>
@@ -1749,7 +1753,11 @@
       </c>
       <c r="B21" s="63" t="n"/>
       <c r="C21" s="64" t="n"/>
-      <c r="D21" s="88" t="n"/>
+      <c r="D21" s="88" t="inlineStr">
+        <is>
+          <t>60 DÍAS</t>
+        </is>
+      </c>
       <c r="E21" s="63" t="n"/>
       <c r="F21" s="63" t="n"/>
       <c r="G21" s="64" t="n"/>
@@ -1781,7 +1789,11 @@
       </c>
       <c r="B22" s="63" t="n"/>
       <c r="C22" s="64" t="n"/>
-      <c r="D22" s="88" t="n"/>
+      <c r="D22" s="88" t="inlineStr">
+        <is>
+          <t>12 MESES</t>
+        </is>
+      </c>
       <c r="E22" s="63" t="n"/>
       <c r="F22" s="63" t="n"/>
       <c r="G22" s="64" t="n"/>
@@ -1813,7 +1825,11 @@
       </c>
       <c r="B23" s="63" t="n"/>
       <c r="C23" s="64" t="n"/>
-      <c r="D23" s="88" t="n"/>
+      <c r="D23" s="88" t="inlineStr">
+        <is>
+          <t>CONTRA ENTREGA TOTAL DE LOS BIENES</t>
+        </is>
+      </c>
       <c r="E23" s="63" t="n"/>
       <c r="F23" s="63" t="n"/>
       <c r="G23" s="64" t="n"/>
@@ -1845,7 +1861,11 @@
       </c>
       <c r="B24" s="63" t="n"/>
       <c r="C24" s="64" t="n"/>
-      <c r="D24" s="88" t="n"/>
+      <c r="D24" s="88" t="inlineStr">
+        <is>
+          <t>NOS ADHERIMOS A LA METODOLOGIA ESTABLECIDA POR LA ENTIDAD</t>
+        </is>
+      </c>
       <c r="E24" s="63" t="n"/>
       <c r="F24" s="63" t="n"/>
       <c r="G24" s="64" t="n"/>
@@ -1877,7 +1897,11 @@
       </c>
       <c r="B25" s="63" t="n"/>
       <c r="C25" s="64" t="n"/>
-      <c r="D25" s="89" t="n"/>
+      <c r="D25" s="89" t="inlineStr">
+        <is>
+          <t>https://www.compraspublicas.gob.ec/ProcesoContratacion/compras/NCO/NCORegistroDetalle.cpe?&amp;id=LJ_WiUl-CoOPX2sUxQlOJ9qAcYSfLnMYDvihWxcoDEg,&amp;op=0</t>
+        </is>
+      </c>
       <c r="E25" s="63" t="n"/>
       <c r="F25" s="63" t="n"/>
       <c r="G25" s="64" t="n"/>

</xml_diff>